<commit_message>
Include script and data to compute statistical differences with k-hop, GSN, ESAN.
</commit_message>
<xml_diff>
--- a/ResultAnalysis.xlsx
+++ b/ResultAnalysis.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nur/Desktop/PhD/gnn-matlang/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5930ACF5-F5F2-AA47-84B5-B5D9E9D05E16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D5CCE197-13E1-D345-A3F3-2B74D9F06920}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -112,7 +112,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="767" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="769" uniqueCount="58">
   <si>
     <t>experiment</t>
   </si>
@@ -280,6 +280,12 @@
   </si>
   <si>
     <t>is_significative_e5</t>
+  </si>
+  <si>
+    <t>Max std.</t>
+  </si>
+  <si>
+    <t>Median std.</t>
   </si>
 </sst>
 </file>
@@ -3062,10 +3068,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AH35"/>
+  <dimension ref="A1:AH38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="Q26" sqref="G24:Q26"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="H39" sqref="H39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5578,6 +5584,24 @@
       <c r="R35" t="str">
         <f t="shared" si="3"/>
         <v>Yes</v>
+      </c>
+    </row>
+    <row r="37" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="G37" t="s">
+        <v>56</v>
+      </c>
+      <c r="H37">
+        <f>MAX(H2:H35)</f>
+        <v>1.4169973832036999</v>
+      </c>
+    </row>
+    <row r="38" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="G38" t="s">
+        <v>57</v>
+      </c>
+      <c r="H38">
+        <f>MEDIAN(H2:H35)</f>
+        <v>0.73208899095101299</v>
       </c>
     </row>
   </sheetData>

</xml_diff>